<commit_message>
added glosario, fixed resources
</commit_message>
<xml_diff>
--- a/puntos_IBX.xlsx
+++ b/puntos_IBX.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25100" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>"Bajo Rojo"</t>
   </si>
@@ -124,81 +124,6 @@
     <t>R.raw.video15_2_small</t>
   </si>
   <si>
-    <t>)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_01_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_01_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_04_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_05_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_06_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_08_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_08_2a</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_10_1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_11_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_12_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_14_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_14_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_16_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_17_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_17_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_17_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_18_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_20_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_21_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_22_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_22_1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_23_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_24_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> new Resource(.drawable.punto_24_1a</t>
-  </si>
-  <si>
     <t>new Resource(R.drawable.punto_02_1,"")</t>
   </si>
   <si>
@@ -295,13 +220,22 @@
     <t>"Secuencia de estratos sedimentarios"</t>
   </si>
   <si>
-    <t>new Resource(R.drawable.anim01_6, "Los Estratos")</t>
-  </si>
-  <si>
-    <t>new Resource(R.raw.audio1b, "Los Estratos")</t>
-  </si>
-  <si>
-    <t>new Resource(R.drawable.punto_01_1,"1-1 Secuencia de estratos rocosos"), new Resource(R.drawable.punto_01_2,"Estratos de la Formación Junquillal"), new Resource(R.drawable.punto_01_3,"Estratos de la Formación Junquillal")</t>
+    <t>video_name</t>
+  </si>
+  <si>
+    <t>anim_name</t>
+  </si>
+  <si>
+    <t>R.drawable.anim01_6</t>
+  </si>
+  <si>
+    <t>"Los Estratos"</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>new Resource(R.raw.audio1b,"Los Estratos")</t>
   </si>
 </sst>
 </file>
@@ -715,98 +649,98 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A2,",",Sheet2!B2,",null, new GeoPoint(",Sheet2!C2,",",Sheet2!D2,"),",Sheet2!E2,".0d,","new Resource[]{",Sheet3!A2,"},",Sheet2!G2,",new Resource[]{",Sheet2!H2,"},",Sheet2!I2,"));")</f>
-        <v>add(new Punto(1,"Secuencia de estratos sedimentarios",null, new GeoPoint(10.9514833333333,-85.7151),300.0d,new Resource[]{new Resource(R.drawable.punto_01_1,""), new Resource(R.drawable.punto_01_2,""), new Resource(R.drawable.punto_01_3,"")},0,new Resource[]{new Resource(R.raw.audio1b, "Los Estratos")},new Resource(R.drawable.anim01_6, "Los Estratos")));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A2,",",Sheet2!B2,",null, new GeoPoint(",Sheet2!C2,",",Sheet2!D2,"),",Sheet2!E2,".0d,","new Resource[]{",Sheet3!A2,"}, new Resource(",Sheet2!G2,",",Sheet2!H2,"),new Resource[]{",Sheet2!I2,"},new Resource(",Sheet2!J2,",",Sheet2!K2,"));")</f>
+        <v>add(new Punto(1,"Secuencia de estratos sedimentarios",null, new GeoPoint(10.9514833333333,-85.7151),300.0d,new Resource[]{new Resource(R.drawable.punto_01_1,""), new Resource(R.drawable.punto_01_2,""), new Resource(R.drawable.punto_01_3,"")}, new Resource(0,""),new Resource[]{new Resource(R.raw.audio1b,"Los Estratos")},new Resource(R.drawable.anim01_6,"Los Estratos"));</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A3,",",Sheet2!B3,",null, new GeoPoint(",Sheet2!C3,",",Sheet2!D3,"),",Sheet2!E3,".0d,","new Resource[]{",Sheet3!A3,"},",Sheet2!G3,",new Resource[]{",Sheet2!H3,"},",Sheet2!I3,"));")</f>
-        <v>add(new Punto(2,"Bajo Rojo",null, new GeoPoint(10.9570833333333,-85.7336333333333),500.0d,new Resource[]{new Resource(R.drawable.punto_02_1,"")},0,new Resource[]{new Resource(R.raw.audio2b, "")},R.drawable.anim02_5));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A3,",",Sheet2!B3,",null, new GeoPoint(",Sheet2!C3,",",Sheet2!D3,"),",Sheet2!E3,".0d,","new Resource[]{",Sheet3!A3,"}, new Resource(",Sheet2!G3,",",Sheet2!H3,"),new Resource[]{",Sheet2!I3,"},new Resource(",Sheet2!J3,",",Sheet2!K3,"));")</f>
+        <v>add(new Punto(2,"Bajo Rojo",null, new GeoPoint(10.9570833333333,-85.7336333333333),500.0d,new Resource[]{new Resource(R.drawable.punto_02_1,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio2b, "")},new Resource(R.drawable.anim02_5,));</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A4,",",Sheet2!B4,",null, new GeoPoint(",Sheet2!C4,",",Sheet2!D4,"),",Sheet2!E4,".0d,","new Resource[]{",Sheet3!A4,"},",Sheet2!G4,",new Resource[]{",Sheet2!H4,"},",Sheet2!I4,"));")</f>
-        <v>add(new Punto(3,"Bahia Junquillal",null, new GeoPoint(10.9698798844808,-85.7271389630961),600.0d,new Resource[]{new Resource(R.drawable.punto_03_1,"")},0,new Resource[]{new Resource(R.raw.audio3b, "")},R.drawable.anim3_4));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A4,",",Sheet2!B4,",null, new GeoPoint(",Sheet2!C4,",",Sheet2!D4,"),",Sheet2!E4,".0d,","new Resource[]{",Sheet3!A4,"}, new Resource(",Sheet2!G4,",",Sheet2!H4,"),new Resource[]{",Sheet2!I4,"},new Resource(",Sheet2!J4,",",Sheet2!K4,"));")</f>
+        <v>add(new Punto(3,"Bahia Junquillal",null, new GeoPoint(10.9698798844808,-85.7271389630961),600.0d,new Resource[]{new Resource(R.drawable.punto_03_1,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio3b, "")},new Resource(R.drawable.anim3_4,));</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A5,",",Sheet2!B5,",null, new GeoPoint(",Sheet2!C5,",",Sheet2!D5,"),",Sheet2!E5,".0d,","new Resource[]{",Sheet3!A5,"},",Sheet2!G5,",new Resource[]{",Sheet2!H5,"},",Sheet2!I5,"));")</f>
-        <v>add(new Punto(4,"Isla Muñecos",null, new GeoPoint(10.9777046049834,-85.7178071072068),200.0d,new Resource[]{new Resource(R.drawable.punto_04_1,""), new Resource(R.drawable.punto_04_3,"")},0,new Resource[]{new Resource(R.raw.audio4b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A5,",",Sheet2!B5,",null, new GeoPoint(",Sheet2!C5,",",Sheet2!D5,"),",Sheet2!E5,".0d,","new Resource[]{",Sheet3!A5,"}, new Resource(",Sheet2!G5,",",Sheet2!H5,"),new Resource[]{",Sheet2!I5,"},new Resource(",Sheet2!J5,",",Sheet2!K5,"));")</f>
+        <v>add(new Punto(4,"Isla Muñecos",null, new GeoPoint(10.9777046049834,-85.7178071072068),200.0d,new Resource[]{new Resource(R.drawable.punto_04_1,""), new Resource(R.drawable.punto_04_3,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio4b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A6,",",Sheet2!B6,",null, new GeoPoint(",Sheet2!C6,",",Sheet2!D6,"),",Sheet2!E6,".0d,","new Resource[]{",Sheet3!A6,"},",Sheet2!G6,",new Resource[]{",Sheet2!H6,"},",Sheet2!I6,"));")</f>
-        <v>add(new Punto(5,"Punto 5",null, new GeoPoint(10.98176182858,-85.7177965097929),50.0d,new Resource[]{new Resource(R.drawable.punto_05_1,""), new Resource(R.drawable.punto_05_2,"")},0,new Resource[]{new Resource(R.raw.audio5b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A6,",",Sheet2!B6,",null, new GeoPoint(",Sheet2!C6,",",Sheet2!D6,"),",Sheet2!E6,".0d,","new Resource[]{",Sheet3!A6,"}, new Resource(",Sheet2!G6,",",Sheet2!H6,"),new Resource[]{",Sheet2!I6,"},new Resource(",Sheet2!J6,",",Sheet2!K6,"));")</f>
+        <v>add(new Punto(5,"Punto 5",null, new GeoPoint(10.98176182858,-85.7177965097929),50.0d,new Resource[]{new Resource(R.drawable.punto_05_1,""), new Resource(R.drawable.punto_05_2,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio5b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A7,",",Sheet2!B7,",null, new GeoPoint(",Sheet2!C7,",",Sheet2!D7,"),",Sheet2!E7,".0d,","new Resource[]{",Sheet3!A7,"},",Sheet2!G7,",new Resource[]{",Sheet2!H7,"},",Sheet2!I7,"));")</f>
-        <v>add(new Punto(6,"Punto 6",null, new GeoPoint(10.9821743821365,-85.7190790800442),50.0d,new Resource[]{new Resource(R.drawable.punto_06_1,""), new Resource(R.drawable.punto_06_2,"")},R.raw.video6_3_small,new Resource[]{new Resource(R.raw.audio6b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A7,",",Sheet2!B7,",null, new GeoPoint(",Sheet2!C7,",",Sheet2!D7,"),",Sheet2!E7,".0d,","new Resource[]{",Sheet3!A7,"}, new Resource(",Sheet2!G7,",",Sheet2!H7,"),new Resource[]{",Sheet2!I7,"},new Resource(",Sheet2!J7,",",Sheet2!K7,"));")</f>
+        <v>add(new Punto(6,"Punto 6",null, new GeoPoint(10.9821743821365,-85.7190790800442),50.0d,new Resource[]{new Resource(R.drawable.punto_06_1,""), new Resource(R.drawable.punto_06_2,"")}, new Resource(R.raw.video6_3_small,),new Resource[]{new Resource(R.raw.audio6b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A8,",",Sheet2!B8,",null, new GeoPoint(",Sheet2!C8,",",Sheet2!D8,"),",Sheet2!E8,".0d,","new Resource[]{",Sheet3!A8,"},",Sheet2!G8,",new Resource[]{",Sheet2!H8,"},",Sheet2!I8,"));")</f>
-        <v>add(new Punto(7,"Punto 7",null, new GeoPoint(10.9839,-85.7189),50.0d,new Resource[]{new Resource(R.drawable.punto_07_1,"")},0,new Resource[]{new Resource(R.raw.audio7b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A8,",",Sheet2!B8,",null, new GeoPoint(",Sheet2!C8,",",Sheet2!D8,"),",Sheet2!E8,".0d,","new Resource[]{",Sheet3!A8,"}, new Resource(",Sheet2!G8,",",Sheet2!H8,"),new Resource[]{",Sheet2!I8,"},new Resource(",Sheet2!J8,",",Sheet2!K8,"));")</f>
+        <v>add(new Punto(7,"Punto 7",null, new GeoPoint(10.9839,-85.7189),50.0d,new Resource[]{new Resource(R.drawable.punto_07_1,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio7b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A9,",",Sheet2!B9,",null, new GeoPoint(",Sheet2!C9,",",Sheet2!D9,"),",Sheet2!E9,".0d,","new Resource[]{",Sheet3!A9,"},",Sheet2!G9,",new Resource[]{",Sheet2!H9,"},",Sheet2!I9,"));")</f>
-        <v>add(new Punto(8,"Punto 8",null, new GeoPoint(11.0016833333333,-85.748105),200.0d,new Resource[]{new Resource(R.drawable.punto_08_1,""), new Resource(R.drawable.punto_08_2,""), new Resource(R.drawable.punto_08_2a,"")},R.raw.video8_3_small,new Resource[]{new Resource(R.raw.audio8b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A9,",",Sheet2!B9,",null, new GeoPoint(",Sheet2!C9,",",Sheet2!D9,"),",Sheet2!E9,".0d,","new Resource[]{",Sheet3!A9,"}, new Resource(",Sheet2!G9,",",Sheet2!H9,"),new Resource[]{",Sheet2!I9,"},new Resource(",Sheet2!J9,",",Sheet2!K9,"));")</f>
+        <v>add(new Punto(8,"Punto 8",null, new GeoPoint(11.0016833333333,-85.748105),200.0d,new Resource[]{new Resource(R.drawable.punto_08_1,""), new Resource(R.drawable.punto_08_2,""), new Resource(R.drawable.punto_08_2a,"")}, new Resource(R.raw.video8_3_small,),new Resource[]{new Resource(R.raw.audio8b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A10,",",Sheet2!B10,",null, new GeoPoint(",Sheet2!C10,",",Sheet2!D10,"),",Sheet2!E10,".0d,","new Resource[]{",Sheet3!A10,"},",Sheet2!G10,",new Resource[]{",Sheet2!H10,"},",Sheet2!I10,"));")</f>
-        <v>add(new Punto(9,"Punto 9",null, new GeoPoint(11.0361333333333,-85.7485833333333),500.0d,new Resource[]{new Resource(R.drawable.punto_09_1,"")},R.raw.video9_6_small,new Resource[]{new Resource(R.raw.audio9b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A10,",",Sheet2!B10,",null, new GeoPoint(",Sheet2!C10,",",Sheet2!D10,"),",Sheet2!E10,".0d,","new Resource[]{",Sheet3!A10,"}, new Resource(",Sheet2!G10,",",Sheet2!H10,"),new Resource[]{",Sheet2!I10,"},new Resource(",Sheet2!J10,",",Sheet2!K10,"));")</f>
+        <v>add(new Punto(9,"Punto 9",null, new GeoPoint(11.0361333333333,-85.7485833333333),500.0d,new Resource[]{new Resource(R.drawable.punto_09_1,"")}, new Resource(R.raw.video9_6_small,),new Resource[]{new Resource(R.raw.audio9b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A11,",",Sheet2!B11,",null, new GeoPoint(",Sheet2!C11,",",Sheet2!D11,"),",Sheet2!E11,".0d,","new Resource[]{",Sheet3!A11,"},",Sheet2!G11,",new Resource[]{",Sheet2!H11,"},",Sheet2!I11,"));")</f>
-        <v>add(new Punto(10,"Punto 10",null, new GeoPoint(11.0381333333333,-85.7387166666666),100.0d,new Resource[]{new Resource(R.drawable.punto_10_1,""), new Resource(R.drawable.punto_10_1a,"")},0,new Resource[]{new Resource(R.raw.audio10b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A11,",",Sheet2!B11,",null, new GeoPoint(",Sheet2!C11,",",Sheet2!D11,"),",Sheet2!E11,".0d,","new Resource[]{",Sheet3!A11,"}, new Resource(",Sheet2!G11,",",Sheet2!H11,"),new Resource[]{",Sheet2!I11,"},new Resource(",Sheet2!J11,",",Sheet2!K11,"));")</f>
+        <v>add(new Punto(10,"Punto 10",null, new GeoPoint(11.0381333333333,-85.7387166666666),100.0d,new Resource[]{new Resource(R.drawable.punto_10_1,""), new Resource(R.drawable.punto_10_1a,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio10b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A12,",",Sheet2!B12,",null, new GeoPoint(",Sheet2!C12,",",Sheet2!D12,"),",Sheet2!E12,".0d,","new Resource[]{",Sheet3!A12,"},",Sheet2!G12,",new Resource[]{",Sheet2!H12,"},",Sheet2!I12,"));")</f>
-        <v>add(new Punto(11,"Punto 11",null, new GeoPoint(11.0448166666666,-85.7417),200.0d,new Resource[]{new Resource(R.drawable.punto_11_1,""), new Resource(R.drawable.punto_11_2,"")},0,new Resource[]{new Resource(R.raw.audio11b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A12,",",Sheet2!B12,",null, new GeoPoint(",Sheet2!C12,",",Sheet2!D12,"),",Sheet2!E12,".0d,","new Resource[]{",Sheet3!A12,"}, new Resource(",Sheet2!G12,",",Sheet2!H12,"),new Resource[]{",Sheet2!I12,"},new Resource(",Sheet2!J12,",",Sheet2!K12,"));")</f>
+        <v>add(new Punto(11,"Punto 11",null, new GeoPoint(11.0448166666666,-85.7417),200.0d,new Resource[]{new Resource(R.drawable.punto_11_1,""), new Resource(R.drawable.punto_11_2,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio11b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A13,",",Sheet2!B13,",null, new GeoPoint(",Sheet2!C13,",",Sheet2!D13,"),",Sheet2!E13,".0d,","new Resource[]{",Sheet3!A13,"},",Sheet2!G13,",new Resource[]{",Sheet2!H13,"},",Sheet2!I13,"));")</f>
-        <v>add(new Punto(12,"Punto 12",null, new GeoPoint(11.0462333333333,-85.7380666666666),200.0d,new Resource[]{new Resource(R.drawable.punto_12_1,""), new Resource(R.drawable.punto_12_2,"")},0,new Resource[]{new Resource(R.raw.audio12b, "")},R.drawable.anim12_3));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A13,",",Sheet2!B13,",null, new GeoPoint(",Sheet2!C13,",",Sheet2!D13,"),",Sheet2!E13,".0d,","new Resource[]{",Sheet3!A13,"}, new Resource(",Sheet2!G13,",",Sheet2!H13,"),new Resource[]{",Sheet2!I13,"},new Resource(",Sheet2!J13,",",Sheet2!K13,"));")</f>
+        <v>add(new Punto(12,"Punto 12",null, new GeoPoint(11.0462333333333,-85.7380666666666),200.0d,new Resource[]{new Resource(R.drawable.punto_12_1,""), new Resource(R.drawable.punto_12_2,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio12b, "")},new Resource(R.drawable.anim12_3,));</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A14,",",Sheet2!B14,",null, new GeoPoint(",Sheet2!C14,",",Sheet2!D14,"),",Sheet2!E14,".0d,","new Resource[]{",Sheet3!A14,"},",Sheet2!G14,",new Resource[]{",Sheet2!H14,"},",Sheet2!I14,"));")</f>
-        <v>add(new Punto(13,"Punto 13",null, new GeoPoint(11.0488333333333,-85.7266666666666),100.0d,new Resource[]{new Resource(R.drawable.punto_13_1,"")},0,new Resource[]{new Resource(R.raw.audio13b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A14,",",Sheet2!B14,",null, new GeoPoint(",Sheet2!C14,",",Sheet2!D14,"),",Sheet2!E14,".0d,","new Resource[]{",Sheet3!A14,"}, new Resource(",Sheet2!G14,",",Sheet2!H14,"),new Resource[]{",Sheet2!I14,"},new Resource(",Sheet2!J14,",",Sheet2!K14,"));")</f>
+        <v>add(new Punto(13,"Punto 13",null, new GeoPoint(11.0488333333333,-85.7266666666666),100.0d,new Resource[]{new Resource(R.drawable.punto_13_1,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio13b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A15,",",Sheet2!B15,",null, new GeoPoint(",Sheet2!C15,",",Sheet2!D15,"),",Sheet2!E15,".0d,","new Resource[]{",Sheet3!A15,"},",Sheet2!G15,",new Resource[]{",Sheet2!H15,"},",Sheet2!I15,"));")</f>
-        <v>add(new Punto(14,"Punto 14",null, new GeoPoint(11.0457666666666,-85.7219),200.0d,new Resource[]{new Resource(R.drawable.punto_14_1,""), new Resource(R.drawable.punto_14_2,""), new Resource(R.drawable.punto_14_3,"")},R.raw.video14_4_small,new Resource[]{new Resource(R.raw.audio14b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A15,",",Sheet2!B15,",null, new GeoPoint(",Sheet2!C15,",",Sheet2!D15,"),",Sheet2!E15,".0d,","new Resource[]{",Sheet3!A15,"}, new Resource(",Sheet2!G15,",",Sheet2!H15,"),new Resource[]{",Sheet2!I15,"},new Resource(",Sheet2!J15,",",Sheet2!K15,"));")</f>
+        <v>add(new Punto(14,"Punto 14",null, new GeoPoint(11.0457666666666,-85.7219),200.0d,new Resource[]{new Resource(R.drawable.punto_14_1,""), new Resource(R.drawable.punto_14_2,""), new Resource(R.drawable.punto_14_3,"")}, new Resource(R.raw.video14_4_small,),new Resource[]{new Resource(R.raw.audio14b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A16,",",Sheet2!B16,",null, new GeoPoint(",Sheet2!C16,",",Sheet2!D16,"),",Sheet2!E16,".0d,","new Resource[]{",Sheet3!A16,"},",Sheet2!G16,",new Resource[]{",Sheet2!H16,"},",Sheet2!I16,"));")</f>
-        <v>add(new Punto(15,"Punto 15",null, new GeoPoint(11.0466881500087,-85.7075191718204),100.0d,new Resource[]{new Resource(R.drawable.punto_15_1,""), new Resource(R.drawable.punto_16_1,""), new Resource(R.drawable.punto_17_1,""), new Resource(R.drawable.punto_17_2,""), new Resource(R.drawable.punto_17_3,""), new Resource(R.drawable.punto_18_1,"")},R.raw.video15_2_small,new Resource[]{new Resource(R.raw.audio17b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A16,",",Sheet2!B16,",null, new GeoPoint(",Sheet2!C16,",",Sheet2!D16,"),",Sheet2!E16,".0d,","new Resource[]{",Sheet3!A16,"}, new Resource(",Sheet2!G16,",",Sheet2!H16,"),new Resource[]{",Sheet2!I16,"},new Resource(",Sheet2!J16,",",Sheet2!K16,"));")</f>
+        <v>add(new Punto(15,"Punto 15",null, new GeoPoint(11.0466881500087,-85.7075191718204),100.0d,new Resource[]{new Resource(R.drawable.punto_15_1,""), new Resource(R.drawable.punto_16_1,""), new Resource(R.drawable.punto_17_1,""), new Resource(R.drawable.punto_17_2,""), new Resource(R.drawable.punto_17_3,""), new Resource(R.drawable.punto_18_1,"")}, new Resource(R.raw.video15_2_small,),new Resource[]{new Resource(R.raw.audio17b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>CONCATENATE("add(new Punto(",Sheet2!A17,",",Sheet2!B17,",null, new GeoPoint(",Sheet2!C17,",",Sheet2!D17,"),",Sheet2!E17,".0d,","new Resource[]{",Sheet3!A17,"},",Sheet2!G17,",new Resource[]{",Sheet2!H17,"},",Sheet2!I17,"));")</f>
-        <v>add(new Punto(19,"Punto 16",null, new GeoPoint(11.0491333333333,-85.7074666666666),50.0d,new Resource[]{new Resource(R.drawable.punto_19_1,""), new Resource(R.drawable.punto_20_1,""), new Resource(R.drawable.punto_21_1,""), new Resource(R.drawable.punto_22_1,""), new Resource(R.drawable.punto_22_1a,""), new Resource(R.drawable.punto_23_1,""), new Resource(R.drawable.punto_24_1,""), new Resource(R.drawable.punto_24_1a,"")},0,new Resource[]{new Resource(R.raw.audio19b,new Resource(R.raw.audio19_1b, ""),new Resource(R.raw.audio19_2b, ""),new Resource(R.raw.audio19_3b, ""),new Resource(R.raw.audio19_4b, ""),new Resource(R.raw.audio19_5b, "")},0));</v>
+        <f>CONCATENATE("add(new Punto(",Sheet2!A17,",",Sheet2!B17,",null, new GeoPoint(",Sheet2!C17,",",Sheet2!D17,"),",Sheet2!E17,".0d,","new Resource[]{",Sheet3!A17,"}, new Resource(",Sheet2!G17,",",Sheet2!H17,"),new Resource[]{",Sheet2!I17,"},new Resource(",Sheet2!J17,",",Sheet2!K17,"));")</f>
+        <v>add(new Punto(19,"Punto 16",null, new GeoPoint(11.0491333333333,-85.7074666666666),50.0d,new Resource[]{new Resource(R.drawable.punto_19_1,""), new Resource(R.drawable.punto_20_1,""), new Resource(R.drawable.punto_21_1,""), new Resource(R.drawable.punto_22_1,""), new Resource(R.drawable.punto_22_1a,""), new Resource(R.drawable.punto_23_1,""), new Resource(R.drawable.punto_24_1,""), new Resource(R.drawable.punto_24_1a,"")}, new Resource(0,),new Resource[]{new Resource(R.raw.audio19b,new Resource(R.raw.audio19_1b, ""),new Resource(R.raw.audio19_2b, ""),new Resource(R.raw.audio19_3b, ""),new Resource(R.raw.audio19_4b, ""),new Resource(R.raw.audio19_5b, "")},new Resource(0,));</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="17" x14ac:dyDescent="0.2">
@@ -916,17 +850,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="52.1640625" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="38.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -946,18 +883,24 @@
         <v>22</v>
       </c>
       <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <v>10.9514833333333</v>
@@ -968,20 +911,27 @@
       <c r="E2">
         <v>300</v>
       </c>
-      <c r="F2" t="s">
-        <v>90</v>
+      <c r="F2" t="str">
+        <f>Sheet3!A2</f>
+        <v>new Resource(R.drawable.punto_01_1,""), new Resource(R.drawable.punto_01_2,""), new Resource(R.drawable.punto_01_3,"")</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -997,20 +947,21 @@
       <c r="E3">
         <v>500</v>
       </c>
-      <c r="F3" t="s">
-        <v>56</v>
+      <c r="F3" t="str">
+        <f>Sheet3!A3</f>
+        <v>new Resource(R.drawable.punto_02_1,"")</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
       <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1026,20 +977,21 @@
       <c r="E4">
         <v>600</v>
       </c>
-      <c r="F4" t="s">
-        <v>57</v>
+      <c r="F4" t="str">
+        <f>Sheet3!A4</f>
+        <v>new Resource(R.drawable.punto_03_1,"")</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>62</v>
-      </c>
       <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1055,20 +1007,21 @@
       <c r="E5">
         <v>200</v>
       </c>
-      <c r="F5" t="s">
-        <v>77</v>
+      <c r="F5" t="str">
+        <f>Sheet3!A5</f>
+        <v>new Resource(R.drawable.punto_04_1,""), new Resource(R.drawable.punto_04_3,"")</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1084,20 +1037,21 @@
       <c r="E6">
         <v>50</v>
       </c>
-      <c r="F6" t="s">
-        <v>78</v>
+      <c r="F6" t="str">
+        <f>Sheet3!A6</f>
+        <v>new Resource(R.drawable.punto_05_1,""), new Resource(R.drawable.punto_05_2,"")</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1113,20 +1067,21 @@
       <c r="E7">
         <v>50</v>
       </c>
-      <c r="F7" t="s">
-        <v>79</v>
+      <c r="F7" t="str">
+        <f>Sheet3!A7</f>
+        <v>new Resource(R.drawable.punto_06_1,""), new Resource(R.drawable.punto_06_2,"")</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
       </c>
-      <c r="H7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1142,20 +1097,21 @@
       <c r="E8">
         <v>50</v>
       </c>
-      <c r="F8" t="s">
-        <v>58</v>
+      <c r="F8" t="str">
+        <f>Sheet3!A8</f>
+        <v>new Resource(R.drawable.punto_07_1,"")</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1171,20 +1127,21 @@
       <c r="E9">
         <v>200</v>
       </c>
-      <c r="F9" t="s">
-        <v>80</v>
+      <c r="F9" t="str">
+        <f>Sheet3!A9</f>
+        <v>new Resource(R.drawable.punto_08_1,""), new Resource(R.drawable.punto_08_2,""), new Resource(R.drawable.punto_08_2a,"")</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="H9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1200,20 +1157,21 @@
       <c r="E10">
         <v>500</v>
       </c>
-      <c r="F10" t="s">
-        <v>59</v>
+      <c r="F10" t="str">
+        <f>Sheet3!A10</f>
+        <v>new Resource(R.drawable.punto_09_1,"")</v>
       </c>
       <c r="G10" t="s">
         <v>28</v>
       </c>
-      <c r="H10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1229,20 +1187,21 @@
       <c r="E11">
         <v>100</v>
       </c>
-      <c r="F11" t="s">
-        <v>81</v>
+      <c r="F11" t="str">
+        <f>Sheet3!A11</f>
+        <v>new Resource(R.drawable.punto_10_1,""), new Resource(R.drawable.punto_10_1a,"")</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1258,20 +1217,21 @@
       <c r="E12">
         <v>200</v>
       </c>
-      <c r="F12" t="s">
-        <v>82</v>
+      <c r="F12" t="str">
+        <f>Sheet3!A12</f>
+        <v>new Resource(R.drawable.punto_11_1,""), new Resource(R.drawable.punto_11_2,"")</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1287,20 +1247,21 @@
       <c r="E13">
         <v>200</v>
       </c>
-      <c r="F13" t="s">
-        <v>83</v>
+      <c r="F13" t="str">
+        <f>Sheet3!A13</f>
+        <v>new Resource(R.drawable.punto_12_1,""), new Resource(R.drawable.punto_12_2,"")</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
-        <v>71</v>
-      </c>
       <c r="I13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1316,20 +1277,21 @@
       <c r="E14">
         <v>100</v>
       </c>
-      <c r="F14" t="s">
-        <v>60</v>
+      <c r="F14" t="str">
+        <f>Sheet3!A14</f>
+        <v>new Resource(R.drawable.punto_13_1,"")</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1345,20 +1307,21 @@
       <c r="E15">
         <v>200</v>
       </c>
-      <c r="F15" t="s">
-        <v>84</v>
+      <c r="F15" t="str">
+        <f>Sheet3!A15</f>
+        <v>new Resource(R.drawable.punto_14_1,""), new Resource(R.drawable.punto_14_2,""), new Resource(R.drawable.punto_14_3,"")</v>
       </c>
       <c r="G15" t="s">
         <v>29</v>
       </c>
-      <c r="H15" t="s">
-        <v>73</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1374,20 +1337,21 @@
       <c r="E16">
         <v>100</v>
       </c>
-      <c r="F16" t="s">
-        <v>85</v>
+      <c r="F16" t="str">
+        <f>Sheet3!A16</f>
+        <v>new Resource(R.drawable.punto_15_1,""), new Resource(R.drawable.punto_16_1,""), new Resource(R.drawable.punto_17_1,""), new Resource(R.drawable.punto_17_2,""), new Resource(R.drawable.punto_17_3,""), new Resource(R.drawable.punto_18_1,"")</v>
       </c>
       <c r="G16" t="s">
         <v>30</v>
       </c>
-      <c r="H16" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>19</v>
       </c>
@@ -1403,16 +1367,17 @@
       <c r="E17">
         <v>50</v>
       </c>
-      <c r="F17" t="s">
-        <v>86</v>
+      <c r="F17" t="str">
+        <f>Sheet3!A17</f>
+        <v>new Resource(R.drawable.punto_19_1,""), new Resource(R.drawable.punto_20_1,""), new Resource(R.drawable.punto_21_1,""), new Resource(R.drawable.punto_22_1,""), new Resource(R.drawable.punto_22_1a,""), new Resource(R.drawable.punto_23_1,""), new Resource(R.drawable.punto_24_1,""), new Resource(R.drawable.punto_24_1a,"")</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17" t="s">
-        <v>75</v>
-      </c>
-      <c r="I17">
+      <c r="I17" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17">
         <v>0</v>
       </c>
     </row>
@@ -1423,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q17"/>
+  <dimension ref="A2:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1435,276 +1400,84 @@
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" t="s">
-        <v>31</v>
-      </c>
-      <c r="L16" t="s">
-        <v>48</v>
-      </c>
-      <c r="M16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" t="s">
-        <v>52</v>
-      </c>
-      <c r="K17" t="s">
-        <v>31</v>
-      </c>
-      <c r="L17" t="s">
-        <v>53</v>
-      </c>
-      <c r="M17" t="s">
-        <v>31</v>
-      </c>
-      <c r="N17" t="s">
-        <v>54</v>
-      </c>
-      <c r="O17" t="s">
-        <v>31</v>
-      </c>
-      <c r="P17" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>